<commit_message>
Added boost turn on and off, redid some pins. Function-ized some. System goes to sleep but does not wake up with photo interrupter at this time (it does wake up with timer but that is set to once an hour).
</commit_message>
<xml_diff>
--- a/hardware/bom.xlsx
+++ b/hardware/bom.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Thing</t>
   </si>
@@ -43,12 +42,6 @@
     <t>Adafruit</t>
   </si>
   <si>
-    <t>Level shifter</t>
-  </si>
-  <si>
-    <t>Boost</t>
-  </si>
-  <si>
     <t>Motor  board (Arduino v2)</t>
   </si>
   <si>
@@ -58,17 +51,80 @@
     <t>Photo interrupter</t>
   </si>
   <si>
-    <t>Resistor setting</t>
+    <t>Photo interrupter board</t>
+  </si>
+  <si>
+    <t>The resistor needs to be 1k as we are using a 3.3V power source</t>
+  </si>
+  <si>
+    <t>Note: I'm not listing the header pins or jumper wires here, you may need some if you don't already have a pack</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9299</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9322</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/13231</t>
+  </si>
+  <si>
+    <t>Power button</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/482</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/858</t>
+  </si>
+  <si>
+    <t>Power boost</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/353</t>
+  </si>
+  <si>
+    <t>6600mAh</t>
+  </si>
+  <si>
+    <t>LiPo battery</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/2465</t>
+  </si>
+  <si>
+    <t>The 500C version also works, probably should switch to it</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1438</t>
+  </si>
+  <si>
+    <t>This must be in switch to 3V mode</t>
+  </si>
+  <si>
+    <t>Not yet integrated but likely needed:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,13 +147,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,13 +461,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" style="4" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -415,11 +483,11 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -429,46 +497,140 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="2">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
       </c>
       <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>29.5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Higher res boost schematic, photo of which resistor to remove for power savings. Added motor shield's main chip and updated Adafruit code to put motor into sleep state (saving 3mA) Updated FeedThingSketch to redo feeding if pellet taken while posting to phant
</commit_message>
<xml_diff>
--- a/hardware/bom.xlsx
+++ b/hardware/bom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Thing</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>Not yet integrated but likely needed:</t>
+  </si>
+  <si>
+    <t>NPN BJT transistor</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/521</t>
+  </si>
+  <si>
+    <t>10k Resistors</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/11508</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8980</t>
+  </si>
+  <si>
+    <t>This is a single 1k, could do better to buy an assorted pack.</t>
+  </si>
+  <si>
+    <t>This is a pack of all 10ks, anything large-ish and matched is fine.</t>
   </si>
 </sst>
 </file>
@@ -461,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,27 +624,81 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -628,9 +706,10 @@
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>